<commit_message>
se actualiza barra de navegacion y estilos
</commit_message>
<xml_diff>
--- a/ventas_dia.xlsx
+++ b/ventas_dia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,18 +455,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cocacola</t>
+          <t>AGUA CRISTAL BOT X 300 ML</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>5000</v>
+        <v>825</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -475,24 +475,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-04-20 15:51:47</t>
+          <t>2025-06-21 00:06:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Empanada</t>
+          <t>Desodorante Rexona Men V8 Roll On X 30ml</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -501,24 +501,24 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-04-20 15:51:47</t>
+          <t>2025-06-21 00:06:24</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cocacola</t>
+          <t>CEPILLO DENTAL COLGATE ULTRA PREMIER</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>5000</v>
+        <v>2050</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -527,24 +527,24 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-04-20 16:03:54</t>
+          <t>2025-06-21 00:06:24</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Empanada</t>
+          <t>tomates</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -553,13 +553,13 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-04-20 16:03:54</t>
+          <t>2025-06-21 00:06:24</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -579,24 +579,24 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-04-20 16:05:49</t>
+          <t>2025-06-21 01:39:44</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Empanada</t>
+          <t>Desodorante para Pies Rexona Efficient Original 55 G</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1000</v>
+        <v>8300</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -605,24 +605,24 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-04-20 16:05:49</t>
+          <t>2025-06-21 01:39:44</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cocacola</t>
+          <t>FIBER PRO CLEAN 450g</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>5000</v>
+        <v>30000</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -631,71 +631,227 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-04-20 16:08:00</t>
+          <t>2025-06-21 01:39:44</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Empanada</t>
+          <t>Cocacola</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-21 01:58:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>126</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AGUA CRISTAL BOT X 300 ML</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>825</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-21 01:58:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>127</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Manzana</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-21 01:58:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>128</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Cocacola</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-21 01:59:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>129</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Cocacola</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-21 01:59:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>130</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>escoba</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
         <v>1000</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>efectivo</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2025-04-20 16:08:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-21 15:04:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>131</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>riquillas</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>65000</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-21 15:04:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Resumen del Día</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Total Vendido</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="B18" t="n">
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Productos Vendidos</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="B19" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Número de Ventas</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>8</v>
+      <c r="B20" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>